<commit_message>
Change example to have a locked table for geoweather_conditions
</commit_message>
<xml_diff>
--- a/app/config/tables/geoweather_conditions/forms/geoweather_conditions/geoweather_conditions.xlsx
+++ b/app/config/tables/geoweather_conditions/forms/geoweather_conditions/geoweather_conditions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -860,7 +863,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -936,7 +939,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>